<commit_message>
venti menu was added
</commit_message>
<xml_diff>
--- a/gen.xlsx
+++ b/gen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Genshin_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FDE97A-88D3-49B4-BC59-4F83E9E8225C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF3E5F7-5D73-449C-BF03-05CFF5DD13B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="71">
   <si>
     <t>ID</t>
   </si>
@@ -186,9 +186,6 @@
 МС</t>
   </si>
   <si>
-    <t>Сила атаки — 1900+, Воччтанова — 200% +, МС — 250-300 ед.</t>
-  </si>
-  <si>
     <t>Сборка Хэйдзо</t>
   </si>
   <si>
@@ -231,6 +228,68 @@
   </si>
   <si>
     <t>Изумрудная тень, Хроники Чертогов в пустыне, Странствующий ансамбль / Воспоминания симэнавы, Азартный игрок</t>
+  </si>
+  <si>
+    <t>Сила атаки — 1900+, Восстанова — 200% +, МС — 250-300 ед.</t>
+  </si>
+  <si>
+    <t>Cборка Венти через МС</t>
+  </si>
+  <si>
+    <t>Сборка Венти через крит. урон</t>
+  </si>
+  <si>
+    <t>HP || В доп. статах МС, восстановление энергии %</t>
+  </si>
+  <si>
+    <t>Сила атаки || В доп. статах МС, восстановление энергии %</t>
+  </si>
+  <si>
+    <t>МС || В доп. статах, восстановление энергии %</t>
+  </si>
+  <si>
+    <t>МС — 600-1000 ед., Восстанова — 180-200% (если в команде нет другого Анемо персонажа)</t>
+  </si>
+  <si>
+    <t>HP || В доп. статах Крит. урон / Шанс крит. попадания , МС,
+Восстановление энергии %,
+Сила атаки %</t>
+  </si>
+  <si>
+    <t>Сила атаки || В доп. статах Крит. урон / Шанс крит. попадания,
+МС,
+Восстановление энергии %,
+Сила атаки %</t>
+  </si>
+  <si>
+    <t>МС / Сила атаки|| В доп. статах Крит. урон / Шанс крит. попадания,
+МС,
+Восстановление энергии %,
+Сила атаки %</t>
+  </si>
+  <si>
+    <t>Бонус Анемо урона % || В доп. статах Крит. урон / Шанс крит. попадания,
+МС,
+Восстановление энергии %,
+Сила атаки %</t>
+  </si>
+  <si>
+    <t>|| В доп. статах Крит. урон / Шанс крит. попадания,
+МС,
+Восстановление энергии %,
+Сила атаки %</t>
+  </si>
+  <si>
+    <t>Сила атаки — 1500-1800 ед., МС — 200-300 ед., Восстанова — 180-200% (если в команде нет другого Анемо персонажа)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Элегия погибели,  Бесструнный, Гаснущие сумерки, Церемониальный лук, Боевой лук Фавония, Охотник во тьме, Ода анемонии </t>
+  </si>
+  <si>
+    <t>Элегия погибели, Аква симулякрум, Небесное крыло, Бесструнный, Гаснущие сумерки, Церемониальный лук, Боевой лук Фавония, Охотник во тьме, Ода анемонии</t>
+  </si>
+  <si>
+    <t>Изумрудная тень, Позолоченные сны, Церемония древней знати, Инструктор, Изгнанник</t>
   </si>
 </sst>
 </file>
@@ -554,7 +613,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,7 +787,7 @@
         <v>27</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="K5" s="1"/>
     </row>
@@ -737,31 +796,31 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="K6" s="1"/>
     </row>
@@ -769,50 +828,66 @@
       <c r="A7" s="1">
         <v>7</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" ht="103.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>8</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" ht="103.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -825,16 +900,16 @@
         <v>31</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -850,16 +925,16 @@
         <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -875,16 +950,16 @@
         <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -900,16 +975,16 @@
         <v>31</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -925,16 +1000,16 @@
         <v>31</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -951,13 +1026,13 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -971,13 +1046,13 @@
         <v>31</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -992,7 +1067,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1007,7 +1082,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1022,7 +1097,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1035,7 +1110,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1048,7 +1123,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1060,7 +1135,7 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -1071,7 +1146,7 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J22" s="1"/>
     </row>
@@ -1082,7 +1157,7 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -1091,7 +1166,7 @@
         <v>31</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -1100,7 +1175,7 @@
         <v>31</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1109,7 +1184,7 @@
         <v>31</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
all is done i guess
</commit_message>
<xml_diff>
--- a/gen.xlsx
+++ b/gen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Genshin_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF00162F-07B9-4D9D-815B-BBE99AE2F58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDD82A8-AF4D-475C-81ED-8EC86B99BE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="636">
   <si>
     <t>ID</t>
   </si>
@@ -1051,9 +1051,6 @@
     <t>МС — 250+ ед., Сила атаки — 1600+, Восстановление энергии — 130%</t>
   </si>
   <si>
-    <t>Сборка дендро Путешественника второстепенного дд</t>
-  </si>
-  <si>
     <t>Воспоминания дремучего леса, Позолоченные сны, Эмблема рассеченной судьбы, Изгнанник</t>
   </si>
   <si>
@@ -1996,18 +1993,35 @@
   </si>
   <si>
     <t>Бонус Гео урона %|| В доп. статах</t>
+  </si>
+  <si>
+    <t>Сборка Элой</t>
+  </si>
+  <si>
+    <t>Сборка дендро Путешественника/цы второстепенного дд</t>
+  </si>
+  <si>
+    <t>Сборка Кирары</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2060,16 +2074,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2353,8 +2370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J57" sqref="J57"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3643,32 +3660,32 @@
       <c r="A41" s="2">
         <v>41</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="4" t="s">
+        <v>634</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="H41" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="I41" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="I41" s="2" t="s">
+      <c r="J41" s="2" t="s">
         <v>330</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -3676,31 +3693,31 @@
         <v>42</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="H42" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="J42" s="2" t="s">
         <v>336</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3708,31 +3725,31 @@
         <v>43</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="G43" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="H43" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="I43" s="2" t="s">
+      <c r="J43" s="2" t="s">
         <v>344</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3740,31 +3757,31 @@
         <v>44</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="H44" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="I44" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="J44" s="2" t="s">
         <v>353</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -3772,31 +3789,31 @@
         <v>45</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>356</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>357</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>176</v>
       </c>
       <c r="F45" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G45" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="H45" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="I45" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="I45" s="2" t="s">
+      <c r="J45" s="2" t="s">
         <v>361</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -3804,60 +3821,60 @@
         <v>46</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>364</v>
-      </c>
       <c r="D46" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>176</v>
       </c>
       <c r="F46" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="G46" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="H46" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="I46" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="I46" s="2" t="s">
+      <c r="J46" s="2" t="s">
         <v>368</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>47</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>370</v>
+      <c r="B47" s="4" t="s">
+        <v>369</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>176</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H47" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="I47" s="2" t="s">
         <v>371</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>372</v>
       </c>
       <c r="J47" s="2"/>
     </row>
@@ -3866,31 +3883,31 @@
         <v>48</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="G48" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="H48" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="I48" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="I48" s="2" t="s">
+      <c r="J48" s="2" t="s">
         <v>380</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3898,31 +3915,31 @@
         <v>49</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>382</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>383</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>248</v>
       </c>
       <c r="E49" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="G49" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="I49" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="G49" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="I49" s="2" t="s">
+      <c r="J49" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -3930,31 +3947,31 @@
         <v>50</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="G50" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="H50" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="H50" s="2" t="s">
+      <c r="I50" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="I50" s="2" t="s">
+      <c r="J50" s="2" t="s">
         <v>395</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -3962,28 +3979,28 @@
         <v>51</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="F51" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="G51" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="H51" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="I51" s="2" t="s">
         <v>403</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>404</v>
       </c>
       <c r="J51" s="2"/>
     </row>
@@ -3992,10 +4009,10 @@
         <v>52</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>405</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>406</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>27</v>
@@ -4013,7 +4030,7 @@
         <v>41</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J52" s="2"/>
     </row>
@@ -4022,31 +4039,31 @@
         <v>53</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="G53" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="H53" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="I53" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="I53" s="2" t="s">
+      <c r="J53" s="2" t="s">
         <v>415</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -4054,31 +4071,31 @@
         <v>54</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="G54" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="G54" s="2" t="s">
+      <c r="H54" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="H54" s="2" t="s">
+      <c r="I54" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="I54" s="2" t="s">
+      <c r="J54" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -4086,31 +4103,31 @@
         <v>55</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="I55" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>427</v>
-      </c>
       <c r="J55" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="259.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -4118,10 +4135,10 @@
         <v>56</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>428</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>429</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>69</v>
@@ -4130,19 +4147,19 @@
         <v>80</v>
       </c>
       <c r="F56" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="G56" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="G56" s="2" t="s">
+      <c r="H56" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="I56" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="I56" s="2" t="s">
+      <c r="J56" s="2" t="s">
         <v>433</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="159" thickBot="1" x14ac:dyDescent="0.35">
@@ -4150,28 +4167,28 @@
         <v>57</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="F57" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="G57" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="G57" s="2" t="s">
+      <c r="H57" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="H57" s="2" t="s">
+      <c r="I57" s="2" t="s">
         <v>441</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>442</v>
       </c>
       <c r="J57" s="2"/>
     </row>
@@ -4180,31 +4197,31 @@
         <v>58</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>88</v>
       </c>
       <c r="D58" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="F58" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="G58" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="G58" s="2" t="s">
+      <c r="H58" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="H58" s="2" t="s">
+      <c r="I58" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="I58" s="2" t="s">
+      <c r="J58" s="2" t="s">
         <v>449</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -4212,28 +4229,28 @@
         <v>59</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>452</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>453</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>266</v>
       </c>
       <c r="F59" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="G59" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="G59" s="2" t="s">
+      <c r="H59" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="I59" s="2" t="s">
         <v>456</v>
-      </c>
-      <c r="I59" s="2" t="s">
-        <v>457</v>
       </c>
       <c r="J59" s="2"/>
     </row>
@@ -4242,31 +4259,31 @@
         <v>60</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="E60" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="F60" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="E60" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="F60" s="2" t="s">
+      <c r="G60" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="G60" s="2" t="s">
+      <c r="H60" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="H60" s="2" t="s">
+      <c r="I60" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="I60" s="2" t="s">
+      <c r="J60" s="2" t="s">
         <v>464</v>
-      </c>
-      <c r="J60" s="2" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="159" thickBot="1" x14ac:dyDescent="0.35">
@@ -4274,31 +4291,31 @@
         <v>61</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="D61" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="F61" s="2" t="s">
+      <c r="G61" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="H61" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="I61" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="H61" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="I61" s="2" t="s">
+      <c r="J61" s="2" t="s">
         <v>470</v>
-      </c>
-      <c r="J61" s="2" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -4306,31 +4323,31 @@
         <v>62</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="F62" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="F62" s="2" t="s">
+      <c r="G62" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="H62" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="H62" s="2" t="s">
+      <c r="I62" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="I62" s="2" t="s">
+      <c r="J62" s="2" t="s">
         <v>479</v>
-      </c>
-      <c r="J62" s="2" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -4338,7 +4355,7 @@
         <v>63</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
@@ -4348,10 +4365,10 @@
         <v>106</v>
       </c>
       <c r="F63" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="G63" s="2" t="s">
         <v>482</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>483</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>217</v>
@@ -4364,7 +4381,7 @@
         <v>64</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
@@ -4383,7 +4400,7 @@
         <v>41</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="J64" s="2"/>
     </row>
@@ -4392,31 +4409,31 @@
         <v>65</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="E65" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="F65" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="G65" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="H65" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="I65" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="H65" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="I65" s="2" t="s">
+      <c r="J65" s="2" t="s">
         <v>492</v>
-      </c>
-      <c r="J65" s="2" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -4424,31 +4441,31 @@
         <v>66</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="E66" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="F66" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="G66" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="H66" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="H66" s="2" t="s">
+      <c r="I66" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="I66" s="2" t="s">
+      <c r="J66" s="2" t="s">
         <v>501</v>
-      </c>
-      <c r="J66" s="2" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -4456,7 +4473,7 @@
         <v>67</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
@@ -4466,10 +4483,10 @@
         <v>106</v>
       </c>
       <c r="F67" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="G67" s="2" t="s">
         <v>504</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>505</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>217</v>
@@ -4482,7 +4499,7 @@
         <v>68</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
@@ -4508,31 +4525,31 @@
         <v>69</v>
       </c>
       <c r="B69" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="D69" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="F69" s="2" t="s">
+      <c r="G69" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="G69" s="2" t="s">
+      <c r="H69" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="H69" s="2" t="s">
+      <c r="I69" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="I69" s="2" t="s">
+      <c r="J69" s="2" t="s">
         <v>512</v>
-      </c>
-      <c r="J69" s="2" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -4540,7 +4557,7 @@
         <v>70</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
@@ -4550,13 +4567,13 @@
         <v>106</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
@@ -4566,31 +4583,31 @@
         <v>71</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="E71" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="F71" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="G71" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="G71" s="2" t="s">
+      <c r="H71" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="H71" s="2" t="s">
+      <c r="I71" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="I71" s="2" t="s">
+      <c r="J71" s="2" t="s">
         <v>523</v>
-      </c>
-      <c r="J71" s="2" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -4598,31 +4615,31 @@
         <v>72</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="E72" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="F72" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="G72" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="G72" s="2" t="s">
+      <c r="H72" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="H72" s="2" t="s">
+      <c r="I72" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="I72" s="2" t="s">
+      <c r="J72" s="2" t="s">
         <v>532</v>
-      </c>
-      <c r="J72" s="2" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -4630,7 +4647,7 @@
         <v>73</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
@@ -4656,31 +4673,31 @@
         <v>74</v>
       </c>
       <c r="B74" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="E74" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="F74" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="G74" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="H74" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="I74" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="H74" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="I74" s="2" t="s">
+      <c r="J74" s="2" t="s">
         <v>541</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="202.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4688,31 +4705,31 @@
         <v>75</v>
       </c>
       <c r="B75" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="D75" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="C75" s="2" t="s">
-        <v>536</v>
-      </c>
-      <c r="D75" s="2" t="s">
+      <c r="E75" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="F75" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="G75" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="H75" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="J75" s="2" t="s">
         <v>547</v>
-      </c>
-      <c r="H75" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>541</v>
-      </c>
-      <c r="J75" s="2" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -4720,31 +4737,31 @@
         <v>76</v>
       </c>
       <c r="B76" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="E76" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="F76" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="G76" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="H76" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="G76" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="H76" s="2" t="s">
+      <c r="I76" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="I76" s="2" t="s">
+      <c r="J76" s="2" t="s">
         <v>555</v>
-      </c>
-      <c r="J76" s="2" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -4752,31 +4769,31 @@
         <v>77</v>
       </c>
       <c r="B77" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="D77" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="F77" s="2" t="s">
+      <c r="G77" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="G77" s="2" t="s">
+      <c r="H77" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="H77" s="2" t="s">
+      <c r="I77" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="I77" s="2" t="s">
+      <c r="J77" s="2" t="s">
         <v>562</v>
-      </c>
-      <c r="J77" s="2" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -4784,28 +4801,28 @@
         <v>78</v>
       </c>
       <c r="B78" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="E78" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="F78" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="G78" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="G78" s="2" t="s">
+      <c r="H78" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="H78" s="2" t="s">
+      <c r="I78" s="2" t="s">
         <v>570</v>
-      </c>
-      <c r="I78" s="2" t="s">
-        <v>571</v>
       </c>
       <c r="J78" s="2"/>
     </row>
@@ -4814,31 +4831,31 @@
         <v>79</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="F79" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="G79" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="G79" s="2" t="s">
+      <c r="H79" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="H79" s="2" t="s">
+      <c r="I79" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="I79" s="2" t="s">
+      <c r="J79" s="2" t="s">
         <v>579</v>
-      </c>
-      <c r="J79" s="2" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -4846,7 +4863,7 @@
         <v>80</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2" t="s">
@@ -4856,13 +4873,13 @@
         <v>106</v>
       </c>
       <c r="F80" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="G80" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="G80" s="2" t="s">
+      <c r="H80" s="2" t="s">
         <v>583</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>584</v>
       </c>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
@@ -4872,31 +4889,31 @@
         <v>81</v>
       </c>
       <c r="B81" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="E81" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="F81" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="G81" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="G81" s="2" t="s">
+      <c r="H81" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="H81" s="2" t="s">
+      <c r="I81" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="I81" s="2" t="s">
+      <c r="J81" s="2" t="s">
         <v>592</v>
-      </c>
-      <c r="J81" s="2" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -4904,31 +4921,31 @@
         <v>82</v>
       </c>
       <c r="B82" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="D82" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="I82" s="2" t="s">
         <v>595</v>
       </c>
-      <c r="D82" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>589</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>590</v>
-      </c>
-      <c r="H82" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="I82" s="2" t="s">
+      <c r="J82" s="2" t="s">
         <v>596</v>
-      </c>
-      <c r="J82" s="2" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -4936,31 +4953,31 @@
         <v>83</v>
       </c>
       <c r="B83" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="E83" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="E83" s="2" t="s">
+      <c r="F83" s="2" t="s">
         <v>601</v>
       </c>
-      <c r="F83" s="2" t="s">
+      <c r="G83" s="2" t="s">
         <v>602</v>
       </c>
-      <c r="G83" s="2" t="s">
+      <c r="H83" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="H83" s="2" t="s">
+      <c r="I83" s="2" t="s">
         <v>604</v>
       </c>
-      <c r="I83" s="2" t="s">
+      <c r="J83" s="2" t="s">
         <v>605</v>
-      </c>
-      <c r="J83" s="2" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -4968,31 +4985,31 @@
         <v>84</v>
       </c>
       <c r="B84" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="D84" s="2" t="s">
         <v>608</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="E84" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="E84" s="2" t="s">
+      <c r="F84" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="F84" s="2" t="s">
+      <c r="G84" s="2" t="s">
         <v>611</v>
       </c>
-      <c r="G84" s="2" t="s">
+      <c r="H84" s="2" t="s">
         <v>612</v>
       </c>
-      <c r="H84" s="2" t="s">
+      <c r="I84" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="I84" s="2" t="s">
+      <c r="J84" s="2" t="s">
         <v>614</v>
-      </c>
-      <c r="J84" s="2" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -5000,31 +5017,31 @@
         <v>85</v>
       </c>
       <c r="B85" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>616</v>
       </c>
-      <c r="C85" s="2" t="s">
+      <c r="D85" s="2" t="s">
         <v>617</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="E85" s="2" t="s">
         <v>618</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="F85" s="2" t="s">
         <v>619</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="G85" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="I85" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="G85" s="2" t="s">
-        <v>620</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>620</v>
-      </c>
-      <c r="I85" s="2" t="s">
+      <c r="J85" s="2" t="s">
         <v>621</v>
-      </c>
-      <c r="J85" s="2" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -5032,31 +5049,31 @@
         <v>86</v>
       </c>
       <c r="B86" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>623</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>617</v>
-      </c>
-      <c r="D86" s="2" t="s">
+      <c r="E86" s="2" t="s">
         <v>624</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="F86" s="2" t="s">
         <v>625</v>
       </c>
-      <c r="F86" s="2" t="s">
+      <c r="G86" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="G86" s="2" t="s">
+      <c r="H86" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="H86" s="2" t="s">
+      <c r="I86" s="2" t="s">
         <v>628</v>
       </c>
-      <c r="I86" s="2" t="s">
+      <c r="J86" s="2" t="s">
         <v>629</v>
-      </c>
-      <c r="J86" s="2" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -5064,10 +5081,10 @@
         <v>87</v>
       </c>
       <c r="B87" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>631</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>632</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>27</v>
@@ -5076,10 +5093,10 @@
         <v>106</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>217</v>
@@ -5091,7 +5108,9 @@
       <c r="A88" s="2">
         <v>88</v>
       </c>
-      <c r="B88" s="2"/>
+      <c r="B88" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2" t="s">
         <v>27</v>
@@ -5115,7 +5134,9 @@
       <c r="A89" s="2">
         <v>89</v>
       </c>
-      <c r="B89" s="2"/>
+      <c r="B89" s="4" t="s">
+        <v>635</v>
+      </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2" t="s">
         <v>27</v>
@@ -5160,7 +5181,7 @@
       <c r="J90" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
all menus and buttons are ready
</commit_message>
<xml_diff>
--- a/gen.xlsx
+++ b/gen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Genshin_bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDD82A8-AF4D-475C-81ED-8EC86B99BE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CE5E8A-0E05-4D13-BA35-A013D1C35A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="687">
   <si>
     <t>ID</t>
   </si>
@@ -724,15 +724,6 @@
     <t>Церемония древней знати, Стойкость Миллелита, Рыцарь крови, Бледный огонь</t>
   </si>
   <si>
-    <t>Сила атаки % / Защита|| В доп. статах</t>
-  </si>
-  <si>
-    <t>Бонус физ. урона|| В доп. статах</t>
-  </si>
-  <si>
-    <t>Крит. урон / Шанс крит. попадания || В доп. статах</t>
-  </si>
-  <si>
     <t>Песнь разбитых сосен, Волчья погибель, Небесное величие, Меч драконьей кости, Черногорская бритва, Церемониальный двуручный меч, Двуручный меч Фавония</t>
   </si>
   <si>
@@ -948,12 +939,6 @@
     <t>Моллюск морских красок, Возлюбленная юная дева, Цветок потерянного рая</t>
   </si>
   <si>
-    <t>НР %|| В доп. статах</t>
-  </si>
-  <si>
-    <t>Бонус лечения|| В доп. статах</t>
-  </si>
-  <si>
     <t>Сборка Моны</t>
   </si>
   <si>
@@ -1528,12 +1513,6 @@
     <t>Сборка электро Путешественника/цы</t>
   </si>
   <si>
-    <t>Восстановление энергии || В доп. статах</t>
-  </si>
-  <si>
-    <t>Бонус Электро урона % || В доп. статах</t>
-  </si>
-  <si>
     <t>Сборка Гань Юй</t>
   </si>
   <si>
@@ -1594,12 +1573,6 @@
     <t>Сборка Чунь Юня</t>
   </si>
   <si>
-    <t>Сила атаки %|| В доп. статах</t>
-  </si>
-  <si>
-    <t>Бонус крио урона|| В доп. статах</t>
-  </si>
-  <si>
     <t>Сборка Дионы</t>
   </si>
   <si>
@@ -1625,9 +1598,6 @@
   </si>
   <si>
     <t>Сборка Ци Ци</t>
-  </si>
-  <si>
-    <t>Бонус лечения || В доп. статах</t>
   </si>
   <si>
     <t>Сборка Мики саппорта</t>
@@ -1834,15 +1804,6 @@
     <t>Сборка Ноэль</t>
   </si>
   <si>
-    <t>Защита %|| В доп. статах</t>
-  </si>
-  <si>
-    <t>Бонус гео урона|| В доп. статах</t>
-  </si>
-  <si>
-    <t>Шанс крит. попадания / Крит. урон || В доп. статах</t>
-  </si>
-  <si>
     <t>Сборка Нин Гуан мейн дд</t>
   </si>
   <si>
@@ -1992,9 +1953,6 @@
     <t>Архаичный камень, Конец гладиатора + Воспоминания Симэнавы, Церемония древней знати</t>
   </si>
   <si>
-    <t>Бонус Гео урона %|| В доп. статах</t>
-  </si>
-  <si>
     <t>Сборка Элой</t>
   </si>
   <si>
@@ -2002,18 +1960,225 @@
   </si>
   <si>
     <t>Сборка Кирары</t>
+  </si>
+  <si>
+    <t>Хищник, Бесструнный, Церемониальный лук, Боевой лук Фавония</t>
+  </si>
+  <si>
+    <t>Воспоминания Симэнавы, Заблудший в метели</t>
+  </si>
+  <si>
+    <t>Сила атаки || В доп. статах Крит. урон, Шанс крит. попадания 
+Сила атаки %, МС, НР %</t>
+  </si>
+  <si>
+    <t>HP || В доп. статах Крит. урон, Шанс крит. попадания 
+Сила атаки %, МС, НР %</t>
+  </si>
+  <si>
+    <t>|| В доп. статах Крит. урон, Шанс крит. попадания 
+Сила атаки %, МС, НР %</t>
+  </si>
+  <si>
+    <t>Бонус Крио урона %|| В доп. статах Крит. урон, Шанс крит. попадания 
+Сила атаки %, МС, НР %</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>НР %|| В доп. статах НР %, Сила атаки % / Восстановление энергии %, Крит. урон, Шанс крит. попадания</t>
+  </si>
+  <si>
+    <t>НР %|| В доп. статах НР %, Сила атаки % / Восстановление энергии %, Крит. урон, Шанс крит. Попадания</t>
+  </si>
+  <si>
+    <t>Элегия погибели, Церемониальный лук, Боевой лук Фавония, Лук Амоса, Изогнутый лук</t>
+  </si>
+  <si>
+    <t>Церемония древней знати, Возлюбленная юная дева, Странствующий ансамбль, Заблудший в метели</t>
+  </si>
+  <si>
+    <t>HP || В доп. статах Сила атаки %, Крит. урон, Шанс крит. попадания, Восстановление энергии %, МС</t>
+  </si>
+  <si>
+    <t>Сила атаки || В доп. статах Сила атаки %, Крит. урон, Шанс крит. попадания, Восстановление энергии %, МС</t>
+  </si>
+  <si>
+    <t>Сила атаки %|| В доп. статах Сила атаки %, Крит. урон, Шанс крит. попадания, Восстановление энергии %, МС</t>
+  </si>
+  <si>
+    <t>Бонус Крио урона|| В доп. статах Сила атаки %, Крит. урон, Шанс крит. попадания, Восстановление энергии %, МС</t>
+  </si>
+  <si>
+    <t>Крит. урон / Шанс крит. попадания || В доп. статах Сила атаки %, Крит. урон, Шанс крит. попадания, Восстановление энергии %, МС</t>
+  </si>
+  <si>
+    <t>Небесное величие, Некованный, Волчья погибель, Меч драконьей кости, Черногорская бритва, Благодатный владыка вод, Прототип: Архаичный</t>
+  </si>
+  <si>
+    <t>Заблудший в метели, Конец гладиатора, Встречная комета, Церемония древней знати, Эмблема рассечённой судьбы</t>
+  </si>
+  <si>
+    <t>Бонус Крио урона %|| В доп. статах Крит. урон / Шанс крит. попадания, Сила атаки %, Восстановление энергии</t>
+  </si>
+  <si>
+    <t>|| В доп. статах Крит. урон / Шанс крит. попадания, Сила атаки %, Восстановление энергии</t>
+  </si>
+  <si>
+    <t>Сила атаки || В доп. статах Крит. урон / Шанс крит. попадания, Сила атаки %, Восстановление энергии</t>
+  </si>
+  <si>
+    <t>HP || В доп. статах Крит. урон / Шанс крит. попадания, Сила атаки %, Восстановление энергии</t>
+  </si>
+  <si>
+    <t>HP || В доп. статах Сила атаки %, Крит. урон/Шанс крит. попадания, Восстановление энергии %</t>
+  </si>
+  <si>
+    <t>Сила атаки || В доп. статах Сила атаки %, Крит. урон/Шанс крит. попадания, Восстановление энергии %</t>
+  </si>
+  <si>
+    <t>Сила атаки % / Защита|| В доп. статах Сила атаки %, Крит. урон/Шанс крит. попадания, Восстановление энергии %</t>
+  </si>
+  <si>
+    <t>Бонус физ. урона|| В доп. статах Сила атаки %, Крит. урон/Шанс крит. попадания, Восстановление энергии %</t>
+  </si>
+  <si>
+    <t>Крит. урон / Шанс крит. попадания || В доп. статах Сила атаки %, Крит. урон/Шанс крит. попадания, Восстановление энергии %</t>
+  </si>
+  <si>
+    <t>HP || В доп. статах НР %, Восстановление энергии, НР,  МС</t>
+  </si>
+  <si>
+    <t>Сила атаки || В доп. статах НР %, Восстановление энергии, НР,  МС</t>
+  </si>
+  <si>
+    <t>НР %|| В доп. статах НР %, Восстановление энергии, НР,  МС</t>
+  </si>
+  <si>
+    <t>Бонус лечения|| В доп. статах НР %, Восстановление энергии, НР,  МС</t>
+  </si>
+  <si>
+    <t>Прототип: Янтарь, Эпос о драконоборцах, Кодекс Фавония, Вино и песни</t>
+  </si>
+  <si>
+    <t>HP || В доп. статах Восстановление энергии %, МС, НР %</t>
+  </si>
+  <si>
+    <t>Сила атаки || В доп. статах Восстановление энергии %, МС, НР %</t>
+  </si>
+  <si>
+    <t>Восстановление энергии || В доп. статах Восстановление энергии %, МС, НР %</t>
+  </si>
+  <si>
+    <t>Бонус Электро урона % || В доп. статах Восстановление энергии %, МС, НР %</t>
+  </si>
+  <si>
+    <t>Крит. урон / Шанс крит. попадания || В доп. статах Восстановление энергии %, МС, НР %</t>
+  </si>
+  <si>
+    <t>Клятва свободы, Рассекающий туман, Небесный меч, Церемониальный меч, Стальное жало, Меч Фавония</t>
+  </si>
+  <si>
+    <t>Эмблема рассеченной судьбы, Церемония древней знати, Громогласный рев ярости</t>
+  </si>
+  <si>
+    <t>HP || В доп. статах Сила атаки %, Восстановление энергии, Крит. урон / Шанс крит. попадания</t>
+  </si>
+  <si>
+    <t>Сила атаки || В доп. статах Сила атаки %, Восстановление энергии, Крит. урон / Шанс крит. Попадания</t>
+  </si>
+  <si>
+    <t>Сила атаки %|| В доп. статах Сила атаки %, Восстановление энергии, Крит. урон / Шанс крит. Попадания</t>
+  </si>
+  <si>
+    <t>Бонус лечения || В доп. статах Сила атаки %, Восстановление энергии, Крит. урон / Шанс крит. Попадания</t>
+  </si>
+  <si>
+    <t>Меч Сокола, Небесный меч, Церемониальный меч, Меч Фавония</t>
+  </si>
+  <si>
+    <t>Возлюбленная юная дева, Церемония древней знати, Заблудший в метели, Конец гладиатора</t>
+  </si>
+  <si>
+    <t>HP || В доп. статах Сила атаки %, Крит. урон / Шанс крит. попадания, Защита</t>
+  </si>
+  <si>
+    <t>Сила атаки || В доп. статах Сила атаки %, Крит. урон / Шанс крит. попадания, Защита</t>
+  </si>
+  <si>
+    <t>Защита %|| В доп. статах Сила атаки %, Крит. урон / Шанс крит. попадания, Защита</t>
+  </si>
+  <si>
+    <t>Бонус гео урона|| В доп. статах Сила атаки %, Крит. урон / Шанс крит. попадания, Защита</t>
+  </si>
+  <si>
+    <t>Шанс крит. попадания / Крит. урон || В доп. статах Сила атаки %, Крит. урон / Шанс крит. попадания, Защита</t>
+  </si>
+  <si>
+    <t>Краснорогий камнеруб, Меч драконьей кости, Белая тень, Небесное величие, Черногорская бритва, Двуручный меч Фавония, Прототип: Архаичный</t>
+  </si>
+  <si>
+    <t>Кокон сладких грез, Конец гладиатора, Встречная комета, Архаичный камень</t>
+  </si>
+  <si>
+    <t>HP || В доп. статах Сила атаки %, Крит. урон, Шанс крит. попадания, Восстановление энергии, МС</t>
+  </si>
+  <si>
+    <t>Сила атаки || В доп. статах Сила атаки %, Крит. урон, Шанс крит. попадания, Восстановление энергии, МС</t>
+  </si>
+  <si>
+    <t>Сила атаки %|| В доп. статах Сила атаки %, Крит. урон, Шанс крит. попадания, Восстановление энергии, МС</t>
+  </si>
+  <si>
+    <t>Бонус Гео урона %|| В доп. статах Сила атаки %, Крит. урон, Шанс крит. попадания, Восстановление энергии, МС</t>
+  </si>
+  <si>
+    <t>Крит. урон / Шанс крит. попадания || В доп. статах Сила атаки %, Крит. урон, Шанс крит. попадания, Восстановление энергии, МС</t>
+  </si>
+  <si>
+    <t>Рассекающий туман, Осквернённое желание, Драгоценный омут, Амэнома Кагэути, Черногорский длинный меч</t>
+  </si>
+  <si>
+    <t>HP || В доп. статах HP %, Восстановление энергии %, Крит. урон/Шанс крит. попадания, МС</t>
+  </si>
+  <si>
+    <t>Сила атаки || В доп. статах HP %, Восстановление энергии %, Крит. урон/Шанс крит. попадания, МС</t>
+  </si>
+  <si>
+    <t>НР % / Крит. урон/Шанс крит. попадания|| В доп. статах HP %, Восстановление энергии %, Крит. урон/Шанс крит. попадания, МС</t>
+  </si>
+  <si>
+    <t>НР % / Бонус Дэндро урона|| В доп. статах HP %, Восстановление энергии %, Крит. урон/Шанс крит. попадания, МС</t>
+  </si>
+  <si>
+    <t>НР % / Сила атаки %|| В доп. статах HP %, Восстановление энергии %, Крит. урон/Шанс крит. попадания, МС</t>
+  </si>
+  <si>
+    <t xml:space="preserve">НР — 30000-40000 ед., Восстановление энергии — 160-180 %, Сила атаки — 1500-1800 ед. </t>
+  </si>
+  <si>
+    <t>Ключ Хадж-нисут, Клятва свободы, Церемониальный меч, Меч Фавония, Лунное сияние Ксифоса, Меч Фавония, Церемониальный меч</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2074,16 +2239,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2370,8 +2538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K88" sqref="K88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2742,7 +2910,9 @@
       <c r="I11" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J11" s="2"/>
+      <c r="J11" s="5" t="s">
+        <v>628</v>
+      </c>
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11" ht="103.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2773,7 +2943,9 @@
       <c r="I12" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="J12" s="2"/>
+      <c r="J12" s="5" t="s">
+        <v>628</v>
+      </c>
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" ht="103.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2804,7 +2976,9 @@
       <c r="I13" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="J13" s="2"/>
+      <c r="J13" s="5" t="s">
+        <v>628</v>
+      </c>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="103.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2835,7 +3009,9 @@
       <c r="I14" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="J14" s="2"/>
+      <c r="J14" s="5" t="s">
+        <v>628</v>
+      </c>
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="103.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2866,7 +3042,9 @@
       <c r="I15" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="J15" s="2"/>
+      <c r="J15" s="5" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
@@ -3006,25 +3184,27 @@
       <c r="C20" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F20" s="2" t="s">
+      <c r="D20" s="5" t="s">
+        <v>644</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>645</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>646</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>647</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>648</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="J20" s="2"/>
+      <c r="J20" s="5" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="21" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
@@ -3098,13 +3278,13 @@
         <v>132</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>133</v>
@@ -3148,7 +3328,7 @@
         <v>144</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>145</v>
@@ -3165,7 +3345,7 @@
         <v>165</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>159</v>
@@ -3255,40 +3435,42 @@
         <v>28</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="G28" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="J28" s="2"/>
+      <c r="J28" s="5" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="29" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>29</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>69</v>
@@ -3297,19 +3479,19 @@
         <v>80</v>
       </c>
       <c r="F29" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="J29" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -3317,31 +3499,31 @@
         <v>30</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="H30" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="J30" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3349,31 +3531,31 @@
         <v>31</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="H31" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="G31" s="2" t="s">
+      <c r="J31" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3381,61 +3563,63 @@
         <v>32</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="H32" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="J32" s="2"/>
+      <c r="J32" s="5" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="33" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>33</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="I33" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="J33" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -3443,31 +3627,31 @@
         <v>34</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="F34" s="2" t="s">
+      <c r="I34" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="J34" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -3475,31 +3659,31 @@
         <v>35</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="H35" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="I35" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="J35" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -3507,89 +3691,95 @@
         <v>36</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
+        <v>285</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>650</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>651</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>651</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>652</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="37" spans="1:10" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>37</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="I37" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="J37" s="2"/>
+      <c r="J37" s="5" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="38" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>38</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="I38" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="J38" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -3597,31 +3787,31 @@
         <v>39</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="H39" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="I39" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="J39" s="2" t="s">
         <v>310</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="173.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -3629,31 +3819,31 @@
         <v>40</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>159</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -3661,31 +3851,31 @@
         <v>41</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>634</v>
+        <v>620</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="I41" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="J41" s="2" t="s">
         <v>325</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -3693,31 +3883,31 @@
         <v>42</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="J42" s="2" t="s">
         <v>331</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3725,31 +3915,31 @@
         <v>43</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="J43" s="2" t="s">
         <v>339</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3757,31 +3947,31 @@
         <v>44</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="H44" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="I44" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="J44" s="2" t="s">
         <v>348</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -3789,31 +3979,31 @@
         <v>45</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>176</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -3821,31 +4011,31 @@
         <v>46</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>176</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3853,28 +4043,28 @@
         <v>47</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>176</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="J47" s="2"/>
     </row>
@@ -3883,31 +4073,31 @@
         <v>48</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="H48" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="I48" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="J48" s="2" t="s">
         <v>375</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3915,31 +4105,31 @@
         <v>49</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="J49" s="2" t="s">
         <v>381</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -3947,31 +4137,31 @@
         <v>50</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="H50" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="I50" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="J50" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -3979,28 +4169,28 @@
         <v>51</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="H51" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="I51" s="2" t="s">
         <v>398</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>403</v>
       </c>
       <c r="J51" s="2"/>
     </row>
@@ -4009,10 +4199,10 @@
         <v>52</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>27</v>
@@ -4030,7 +4220,7 @@
         <v>41</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="J52" s="2"/>
     </row>
@@ -4039,31 +4229,31 @@
         <v>53</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="G53" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="H53" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="I53" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="J53" s="2" t="s">
         <v>410</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -4071,31 +4261,31 @@
         <v>54</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G54" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="H54" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="I54" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="J54" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -4103,31 +4293,31 @@
         <v>55</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="H55" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="E55" s="2" t="s">
+      <c r="I55" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="J55" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="259.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -4135,10 +4325,10 @@
         <v>56</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>69</v>
@@ -4147,19 +4337,19 @@
         <v>80</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="159" thickBot="1" x14ac:dyDescent="0.35">
@@ -4167,28 +4357,28 @@
         <v>57</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="G57" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="H57" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="I57" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>441</v>
       </c>
       <c r="J57" s="2"/>
     </row>
@@ -4197,31 +4387,31 @@
         <v>58</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>88</v>
       </c>
       <c r="D58" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="I58" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="J58" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>448</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -4229,28 +4419,28 @@
         <v>59</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="H59" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="I59" s="2" t="s">
         <v>451</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="I59" s="2" t="s">
-        <v>456</v>
       </c>
       <c r="J59" s="2"/>
     </row>
@@ -4259,31 +4449,31 @@
         <v>60</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="H60" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="I60" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="J60" s="2" t="s">
         <v>459</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="I60" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="J60" s="2" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="159" thickBot="1" x14ac:dyDescent="0.35">
@@ -4291,31 +4481,31 @@
         <v>61</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="J61" s="2" t="s">
         <v>465</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="I61" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="J61" s="2" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -4323,117 +4513,127 @@
         <v>62</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="G62" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="H62" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="I62" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="J62" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="F62" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="I62" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="J62" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>63</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
-    </row>
-    <row r="64" spans="1:10" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+        <v>475</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>660</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>656</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>657</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>658</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>64</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>41</v>
+        <v>476</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>643</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>640</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>641</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="J64" s="2"/>
+        <v>477</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="65" spans="1:10" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>65</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="J65" s="2" t="s">
         <v>485</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="I65" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="J65" s="2" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -4441,173 +4641,191 @@
         <v>66</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="I66" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="J66" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>496</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="I66" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="J66" s="2" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:10" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>67</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
-    </row>
-    <row r="68" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>495</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>633</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>634</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>635</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="J67" s="5" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>68</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
+        <v>496</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>632</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>629</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>630</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>629</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>631</v>
+      </c>
+      <c r="J68" s="5" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="69" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>69</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>399</v>
+        <v>393</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>394</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="I69" s="2" t="s">
-        <v>511</v>
+        <v>501</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>502</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>70</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>514</v>
-      </c>
-      <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
+        <v>504</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>666</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>661</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>662</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>663</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>664</v>
+      </c>
+      <c r="I70" s="5" t="s">
+        <v>665</v>
+      </c>
+      <c r="J70" s="5" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="71" spans="1:10" ht="159" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>71</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>515</v>
+        <v>505</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>516</v>
+        <v>506</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>518</v>
+        <v>508</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>521</v>
+        <v>511</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>522</v>
+        <v>512</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -4615,31 +4833,31 @@
         <v>72</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>524</v>
+        <v>514</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>525</v>
+        <v>515</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>527</v>
+        <v>517</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>528</v>
+        <v>518</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>529</v>
+        <v>519</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -4647,7 +4865,7 @@
         <v>73</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2" t="s">
@@ -4666,38 +4884,40 @@
         <v>41</v>
       </c>
       <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
+      <c r="J73" s="2" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="74" spans="1:10" ht="202.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>74</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>539</v>
+        <v>529</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>539</v>
+        <v>529</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>540</v>
+        <v>530</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>541</v>
+        <v>531</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="202.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -4705,31 +4925,31 @@
         <v>75</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>542</v>
+        <v>532</v>
       </c>
       <c r="C75" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="F75" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>545</v>
-      </c>
       <c r="G75" s="2" t="s">
-        <v>546</v>
+        <v>536</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>540</v>
+        <v>530</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -4737,31 +4957,31 @@
         <v>76</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>553</v>
+        <v>543</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>554</v>
+        <v>544</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>555</v>
+        <v>545</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -4769,31 +4989,31 @@
         <v>77</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>556</v>
+        <v>546</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
       <c r="D77" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="H77" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="I77" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="F77" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>559</v>
-      </c>
-      <c r="H77" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="I77" s="2" t="s">
-        <v>561</v>
-      </c>
       <c r="J77" s="2" t="s">
-        <v>562</v>
+        <v>552</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -4801,119 +5021,127 @@
         <v>78</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>563</v>
+        <v>553</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>564</v>
+        <v>554</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>565</v>
+        <v>555</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>566</v>
+        <v>556</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>567</v>
+        <v>557</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>568</v>
+        <v>558</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>569</v>
+        <v>559</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="J78" s="2"/>
+        <v>560</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="79" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>79</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>571</v>
+        <v>561</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>572</v>
+        <v>562</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>573</v>
+        <v>563</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
       <c r="J79" s="2" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>80</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>580</v>
-      </c>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="I80" s="2"/>
-      <c r="J80" s="2"/>
+        <v>570</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>673</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>667</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>668</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>669</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>670</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>671</v>
+      </c>
+      <c r="I80" s="5" t="s">
+        <v>672</v>
+      </c>
+      <c r="J80" s="5" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="81" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>81</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>584</v>
+        <v>571</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>585</v>
+        <v>572</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>586</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>587</v>
+        <v>573</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>574</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>588</v>
+        <v>575</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>589</v>
+        <v>576</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>590</v>
+        <v>577</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>591</v>
+        <v>578</v>
       </c>
       <c r="J81" s="2" t="s">
-        <v>592</v>
+        <v>579</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -4921,31 +5149,31 @@
         <v>82</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>593</v>
+        <v>580</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>594</v>
+        <v>581</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>586</v>
+        <v>573</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>587</v>
+        <v>574</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>588</v>
+        <v>575</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>589</v>
+        <v>576</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>590</v>
+        <v>577</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="J82" s="2" t="s">
-        <v>596</v>
+        <v>583</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -4953,31 +5181,31 @@
         <v>83</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>597</v>
+        <v>584</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>599</v>
+        <v>586</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>600</v>
+        <v>587</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>601</v>
+        <v>588</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>602</v>
+        <v>589</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="J83" s="2" t="s">
-        <v>605</v>
+        <v>592</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -4985,31 +5213,31 @@
         <v>84</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>607</v>
+        <v>594</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>608</v>
+        <v>595</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>609</v>
+        <v>596</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>610</v>
+        <v>597</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>611</v>
+        <v>598</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>612</v>
+        <v>599</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>613</v>
+        <v>600</v>
       </c>
       <c r="J84" s="2" t="s">
-        <v>614</v>
+        <v>601</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -5017,31 +5245,31 @@
         <v>85</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>615</v>
+        <v>602</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>616</v>
+        <v>603</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>618</v>
+        <v>605</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>619</v>
+        <v>606</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>619</v>
+        <v>606</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>619</v>
+        <v>606</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>620</v>
+        <v>607</v>
       </c>
       <c r="J85" s="2" t="s">
-        <v>621</v>
+        <v>608</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -5049,31 +5277,31 @@
         <v>86</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>622</v>
+        <v>609</v>
       </c>
       <c r="C86" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>611</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="J86" s="2" t="s">
         <v>616</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>624</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>625</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>626</v>
-      </c>
-      <c r="H86" s="2" t="s">
-        <v>627</v>
-      </c>
-      <c r="I86" s="2" t="s">
-        <v>628</v>
-      </c>
-      <c r="J86" s="2" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -5081,80 +5309,94 @@
         <v>87</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>630</v>
+        <v>617</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>631</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="H87" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="I87" s="2"/>
-      <c r="J87" s="2"/>
-    </row>
-    <row r="88" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>618</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>674</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>676</v>
+      </c>
+      <c r="G87" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="H87" s="5" t="s">
+        <v>678</v>
+      </c>
+      <c r="I87" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="J87" s="2" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>88</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>633</v>
-      </c>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H88" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I88" s="2"/>
-      <c r="J88" s="2"/>
-    </row>
-    <row r="89" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>619</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>623</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>625</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>626</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>627</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>626</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>622</v>
+      </c>
+      <c r="J88" s="5" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>89</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>635</v>
+        <v>621</v>
       </c>
       <c r="C89" s="2"/>
-      <c r="D89" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G89" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H89" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I89" s="2"/>
-      <c r="J89" s="2"/>
+      <c r="D89" s="5" t="s">
+        <v>680</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>683</v>
+      </c>
+      <c r="H89" s="5" t="s">
+        <v>682</v>
+      </c>
+      <c r="I89" s="5" t="s">
+        <v>686</v>
+      </c>
+      <c r="J89" s="5" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="90" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
@@ -5181,7 +5423,7 @@
       <c r="J90" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>